<commit_message>
Removing accidental temp file
</commit_message>
<xml_diff>
--- a/coding_batches/batch7/batch7_quota_screening_human_examination_of_summarisation_consistency_check.xlsx
+++ b/coding_batches/batch7/batch7_quota_screening_human_examination_of_summarisation_consistency_check.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benke\devEnv\llmproc\coding_batches\batch7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98F31848-F6B0-4D89-864D-51CDC9578112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B76363B-4C2B-4536-B0FE-71A1D63C6A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{C104A3B6-9D09-4FE9-A613-8BAB863A1709}"/>
   </bookViews>
@@ -5796,8 +5796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289AAA27-C637-4A71-83CC-B580EC2C9276}">
   <dimension ref="A1:U528"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>